<commit_message>
add title of the chart in the HW3_Excel1/HW3_113501065.xlsx
</commit_message>
<xml_diff>
--- a/HW3_Excel1/HW3_113501065.xlsx
+++ b/HW3_Excel1/HW3_113501065.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterchiu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E85F0-A5BD-5D45-A322-3C484788B37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63900212-8B63-9742-9405-BBD30CD1D114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{60C2E2F6-AD98-4042-9BF5-DA3DB7B4AD4C}"/>
+    <workbookView xWindow="3200" yWindow="2500" windowWidth="33600" windowHeight="19120" xr2:uid="{60C2E2F6-AD98-4042-9BF5-DA3DB7B4AD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -355,16 +355,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -456,6 +446,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>工作表1!$B$2:$B$15</c:f>
@@ -750,6 +797,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Pass vs Fail Proportion</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -801,6 +874,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-77D1-8D45-B4AE-532C6963349A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -816,6 +894,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-77D1-8D45-B4AE-532C6963349A}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -878,7 +961,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>工作表1!$L$19:$L$20</c:f>
+              <c:f>工作表1!$L$18:$L$19</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -892,7 +975,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$M$19:$M$20</c:f>
+              <c:f>工作表1!$M$18:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -945,7 +1028,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2111,16 +2194,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>340360</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>538480</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1590040</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2149,14 +2232,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>147320</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>416560</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:rowOff>71120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2484,7 +2567,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3157,20 +3240,20 @@
         <v>76.871428571428581</v>
       </c>
     </row>
+    <row r="18" spans="3:13">
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18">
+        <f>COUNTIF(L2:L15,"pass")</f>
+        <v>12</v>
+      </c>
+    </row>
     <row r="19" spans="3:13">
       <c r="L19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M19">
-        <f>COUNTIF(L2:L15,"pass")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13">
-      <c r="L20" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20">
         <f>COUNTIF(L3:L16,"fail")</f>
         <v>2</v>
       </c>
@@ -3183,11 +3266,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="L2:L15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"pass"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>